<commit_message>
refactor code:balanced split of test-train set...
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -511,7 +511,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Florian</t>
+          <t>Aquari</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Mythron</t>
+          <t>Nexoon</t>
         </is>
       </c>
     </row>
@@ -991,7 +991,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Aquari</t>
+          <t>Florian</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Mythron</t>
+          <t>Faerix</t>
         </is>
       </c>
     </row>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Quixnar</t>
+          <t>Zorblax</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Mythron</t>
+          <t>Faerix</t>
         </is>
       </c>
     </row>
@@ -2311,7 +2311,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Quixnar</t>
+          <t>Cybex</t>
         </is>
       </c>
     </row>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Mythron</t>
+          <t>Faerix</t>
         </is>
       </c>
     </row>
@@ -2671,7 +2671,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Emotivor</t>
+          <t>Sentire</t>
         </is>
       </c>
     </row>
@@ -3311,7 +3311,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Aquari</t>
+          <t>Florian</t>
         </is>
       </c>
     </row>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>Sentire</t>
+          <t>Emotivor</t>
         </is>
       </c>
     </row>
@@ -3891,7 +3891,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>Sentire</t>
+          <t>Emotivor</t>
         </is>
       </c>
     </row>
@@ -4511,7 +4511,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>Sentire</t>
+          <t>Emotivor</t>
         </is>
       </c>
     </row>
@@ -4551,7 +4551,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>Faerix</t>
+          <t>Mythron</t>
         </is>
       </c>
     </row>
@@ -4711,7 +4711,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>Quixnar</t>
+          <t>Zorblax</t>
         </is>
       </c>
     </row>
@@ -4891,7 +4891,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>Emotivor</t>
+          <t>Sentire</t>
         </is>
       </c>
     </row>
@@ -4911,7 +4911,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>Cybex</t>
+          <t>Nexoon</t>
         </is>
       </c>
     </row>
@@ -5151,7 +5151,7 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>Cybex</t>
+          <t>Faerix</t>
         </is>
       </c>
     </row>
@@ -5251,7 +5251,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>Quixnar</t>
+          <t>Zorblax</t>
         </is>
       </c>
     </row>
@@ -5851,7 +5851,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Zorblax</t>
+          <t>Quixnar</t>
         </is>
       </c>
     </row>
@@ -5971,7 +5971,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Quixnar</t>
+          <t>Zorblax</t>
         </is>
       </c>
     </row>
@@ -6071,7 +6071,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Sentire</t>
+          <t>Emotivor</t>
         </is>
       </c>
     </row>
@@ -6271,7 +6271,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Quixnar</t>
+          <t>Faerix</t>
         </is>
       </c>
     </row>
@@ -6351,7 +6351,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Faerix</t>
+          <t>Mythron</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor code to handle unknown categories in OneHotEncoder and optimize TF-IDF vectorization...
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -511,7 +511,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Aquari</t>
+          <t>Florian</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Nexoon</t>
+          <t>Mythron</t>
         </is>
       </c>
     </row>
@@ -991,7 +991,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Florian</t>
+          <t>Aquari</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Emotivor</t>
+          <t>Sentire</t>
         </is>
       </c>
     </row>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Emotivor</t>
+          <t>Sentire</t>
         </is>
       </c>
     </row>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Sentire</t>
+          <t>Emotivor</t>
         </is>
       </c>
     </row>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Sentire</t>
+          <t>Emotivor</t>
         </is>
       </c>
     </row>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Quixnar</t>
+          <t>Zorblax</t>
         </is>
       </c>
     </row>
@@ -1651,7 +1651,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Cybex</t>
+          <t>Nexoon</t>
         </is>
       </c>
     </row>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Cybex</t>
+          <t>Nexoon</t>
         </is>
       </c>
     </row>
@@ -2131,7 +2131,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Florian</t>
+          <t>Aquari</t>
         </is>
       </c>
     </row>
@@ -2151,7 +2151,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Cybex</t>
+          <t>Nexoon</t>
         </is>
       </c>
     </row>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Mythron</t>
+          <t>Faerix</t>
         </is>
       </c>
     </row>
@@ -2331,7 +2331,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Quixnar</t>
+          <t>Zorblax</t>
         </is>
       </c>
     </row>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Faerix</t>
+          <t>Mythron</t>
         </is>
       </c>
     </row>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Florian</t>
+          <t>Aquari</t>
         </is>
       </c>
     </row>
@@ -2571,7 +2571,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Zorblax</t>
+          <t>Quixnar</t>
         </is>
       </c>
     </row>
@@ -2671,7 +2671,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Sentire</t>
+          <t>Emotivor</t>
         </is>
       </c>
     </row>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Cybex</t>
+          <t>Nexoon</t>
         </is>
       </c>
     </row>
@@ -3271,7 +3271,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Nexoon</t>
+          <t>Cybex</t>
         </is>
       </c>
     </row>
@@ -3311,7 +3311,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Florian</t>
+          <t>Aquari</t>
         </is>
       </c>
     </row>
@@ -3371,7 +3371,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Aquari</t>
+          <t>Florian</t>
         </is>
       </c>
     </row>
@@ -3471,7 +3471,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Emotivor</t>
+          <t>Florian</t>
         </is>
       </c>
     </row>
@@ -3491,7 +3491,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>Emotivor</t>
+          <t>Nexoon</t>
         </is>
       </c>
     </row>
@@ -3611,7 +3611,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>Emotivor</t>
+          <t>Sentire</t>
         </is>
       </c>
     </row>
@@ -3811,7 +3811,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>Nexoon</t>
+          <t>Cybex</t>
         </is>
       </c>
     </row>
@@ -3891,7 +3891,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>Emotivor</t>
+          <t>Sentire</t>
         </is>
       </c>
     </row>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>Emotivor</t>
+          <t>Sentire</t>
         </is>
       </c>
     </row>
@@ -4091,7 +4091,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>Zorblax</t>
+          <t>Quixnar</t>
         </is>
       </c>
     </row>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>Cybex</t>
+          <t>Nexoon</t>
         </is>
       </c>
     </row>
@@ -4691,7 +4691,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>Faerix</t>
+          <t>Mythron</t>
         </is>
       </c>
     </row>
@@ -4731,7 +4731,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>Cybex</t>
+          <t>Nexoon</t>
         </is>
       </c>
     </row>
@@ -5251,7 +5251,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>Zorblax</t>
+          <t>Quixnar</t>
         </is>
       </c>
     </row>
@@ -5331,7 +5331,7 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>Sentire</t>
+          <t>Emotivor</t>
         </is>
       </c>
     </row>
@@ -5411,7 +5411,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>Emotivor</t>
+          <t>Sentire</t>
         </is>
       </c>
     </row>
@@ -5471,7 +5471,7 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>Quixnar</t>
+          <t>Zorblax</t>
         </is>
       </c>
     </row>
@@ -5671,7 +5671,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Mythron</t>
+          <t>Faerix</t>
         </is>
       </c>
     </row>
@@ -5731,7 +5731,7 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Faerix</t>
+          <t>Mythron</t>
         </is>
       </c>
     </row>
@@ -5851,7 +5851,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Quixnar</t>
+          <t>Zorblax</t>
         </is>
       </c>
     </row>
@@ -5971,7 +5971,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Zorblax</t>
+          <t>Quixnar</t>
         </is>
       </c>
     </row>
@@ -5991,7 +5991,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Quixnar</t>
+          <t>Zorblax</t>
         </is>
       </c>
     </row>
@@ -6071,7 +6071,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Emotivor</t>
+          <t>Sentire</t>
         </is>
       </c>
     </row>
@@ -6351,7 +6351,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Mythron</t>
+          <t>Faerix</t>
         </is>
       </c>
     </row>

</xml_diff>